<commit_message>
update restults and doc
</commit_message>
<xml_diff>
--- a/document/final/results.xlsx
+++ b/document/final/results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t>Training species</t>
   </si>
@@ -110,6 +110,20 @@
   </si>
   <si>
     <t>SVM linear</t>
+  </si>
+  <si>
+    <t>Set threshold to be &gt;= 20 samples per species; K=1000. No resize before SIFT.</t>
+  </si>
+  <si>
+    <t>Set threshold to be &gt;= 20 samples per species; K=3000. No resize before SIFT.</t>
+  </si>
+  <si>
+    <t>factor=3.
+rotation=10.
+shift=0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set threshold to be &gt;= 20 samples per species. Apply histogram normalization and then use K-means to remove background color </t>
   </si>
 </sst>
 </file>
@@ -429,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView zoomScale="182" zoomScaleNormal="182" zoomScalePageLayoutView="182" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -806,10 +820,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="141" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,9 +835,10 @@
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="9.1640625" customWidth="1"/>
     <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="68.6640625" customWidth="1"/>
+    <col min="12" max="12" width="68.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -898,7 +913,7 @@
       <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -937,12 +952,53 @@
         <v>21</v>
       </c>
     </row>
+    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>0.99860000000000004</v>
+      </c>
+      <c r="C4">
+        <v>5678</v>
+      </c>
+      <c r="D4">
+        <v>109</v>
+      </c>
+      <c r="E4">
+        <v>28821</v>
+      </c>
+      <c r="F4">
+        <v>66</v>
+      </c>
+      <c r="G4">
+        <v>1194</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10">
-        <v>0.64049999999999996</v>
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="C10">
+        <v>0.40949999999999998</v>
       </c>
       <c r="D10">
         <v>109</v>
@@ -968,8 +1024,46 @@
       <c r="K10" t="s">
         <v>26</v>
       </c>
-      <c r="L10" t="s">
-        <v>16</v>
+      <c r="L10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>0.86629999999999996</v>
+      </c>
+      <c r="C11">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="D11">
+        <v>109</v>
+      </c>
+      <c r="E11">
+        <v>9607</v>
+      </c>
+      <c r="F11">
+        <v>66</v>
+      </c>
+      <c r="G11">
+        <v>1194</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>